<commit_message>
Landscape and Financials tool update
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ali Salem\Desktop\Slide-Automate-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4704A9B1-0544-4EE3-A7D0-FCC87B71D532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9230663F-B993-469C-8BC3-5DBF969B0BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="24" windowWidth="23016" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="24" windowWidth="23016" windowHeight="12216" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assortment" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="156">
   <si>
     <t>Field</t>
   </si>
@@ -491,6 +491,15 @@
   </si>
   <si>
     <t>RunManuf</t>
+  </si>
+  <si>
+    <t>slides_Period</t>
+  </si>
+  <si>
+    <t>P3M</t>
+  </si>
+  <si>
+    <t>rpvm_comp_brands</t>
   </si>
 </sst>
 </file>
@@ -862,7 +871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
@@ -2786,10 +2795,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9FAF09-08A3-4B91-B541-B6D49B1C84A3}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3278,6 +3287,28 @@
       </c>
       <c r="C41" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>153</v>
+      </c>
+      <c r="B42" t="s">
+        <v>154</v>
+      </c>
+      <c r="C42" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>155</v>
+      </c>
+      <c r="B43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -3841,10 +3872,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC25CABC-59C5-45BC-822F-0F71D7C65392}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C38" sqref="A38:C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4288,6 +4319,17 @@
         <v>39</v>
       </c>
     </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>153</v>
+      </c>
+      <c r="B38" t="s">
+        <v>154</v>
+      </c>
+      <c r="C38" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Promotion, PPA and Pricing tool Update
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ali Salem\Desktop\Slide-Automate-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9230663F-B993-469C-8BC3-5DBF969B0BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3522FB18-0984-4744-ABFC-82792796F4B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="24" windowWidth="23016" windowHeight="12216" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="24" windowWidth="23016" windowHeight="12216" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assortment" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="157">
   <si>
     <t>Field</t>
   </si>
@@ -500,6 +500,9 @@
   </si>
   <si>
     <t>rpvm_comp_brands</t>
+  </si>
+  <si>
+    <t>P12M</t>
   </si>
 </sst>
 </file>
@@ -2272,10 +2275,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6560B172-1B59-487F-ACF4-BA38A1166E57}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C44" sqref="A44:C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2788,6 +2791,17 @@
         <v>43</v>
       </c>
     </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>153</v>
+      </c>
+      <c r="B44" t="s">
+        <v>154</v>
+      </c>
+      <c r="C44" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2797,7 +2811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9FAF09-08A3-4B91-B541-B6D49B1C84A3}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
@@ -3318,10 +3332,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F065A64-70F8-4E29-A57E-BC789E2BC90C}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3864,6 +3878,17 @@
         <v>43</v>
       </c>
     </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>153</v>
+      </c>
+      <c r="B47" t="s">
+        <v>156</v>
+      </c>
+      <c r="C47" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3875,7 +3900,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="C38" sqref="A38:C38"/>
+      <selection activeCell="A38" sqref="A38:C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Promo and Dates param update
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ali Salem\Desktop\Slide-Automate-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78F4E1E-39A2-416F-AA36-03BF7F1F4C8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6076E933-EC64-4C3B-8275-DC79DA706DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="24" windowWidth="23016" windowHeight="12216" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="24" windowWidth="23016" windowHeight="12216" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assortment" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="169">
   <si>
     <t>Field</t>
   </si>
@@ -526,9 +526,6 @@
     <t>Carrefour Hyper + Drive,Carrefour Supermarket + Drive,Carrefour Proximite,Intermarche Super,Intermarche Hyper,Intermarche Proxi</t>
   </si>
   <si>
-    <t>01/08/2022</t>
-  </si>
-  <si>
     <t>'Aperitif': 0.27,'Enfant': 0.35,"Frais A Tartiner" : 0.25,"Ingredient A Chaud" : 0.3,"Salade" : 0.28</t>
   </si>
   <si>
@@ -536,6 +533,12 @@
   </si>
   <si>
     <t>Bel France Dataset</t>
+  </si>
+  <si>
+    <t>2025-07-01</t>
+  </si>
+  <si>
+    <t>2022-07-01</t>
   </si>
 </sst>
 </file>
@@ -905,10 +908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1274,10 +1277,10 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B31" s="4">
-        <v>45748</v>
+        <v>144</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>168</v>
       </c>
       <c r="C31" t="s">
         <v>35</v>
@@ -1285,24 +1288,21 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>66</v>
+        <v>28</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>167</v>
       </c>
       <c r="C32" t="s">
-        <v>43</v>
-      </c>
-      <c r="D32" t="s">
-        <v>73</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>30</v>
-      </c>
-      <c r="B33" s="1" t="b">
-        <v>1</v>
+        <v>29</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="C33" t="s">
         <v>43</v>
@@ -1313,67 +1313,81 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>31</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>136</v>
+        <v>30</v>
+      </c>
+      <c r="B34" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>35</v>
+        <v>43</v>
+      </c>
+      <c r="D34" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" s="6">
-        <v>1000000</v>
+        <v>31</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="C35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
+      </c>
+      <c r="B36" s="6">
+        <v>1000000</v>
       </c>
       <c r="C36" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>33</v>
-      </c>
-      <c r="B37" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C37" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>149</v>
+        <v>33</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="C38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C39" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>148</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1384,10 +1398,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C131E685-1F6A-40C1-B63B-FBE27479E849}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C37"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1750,10 +1764,10 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B31" s="4">
-        <v>45748</v>
+        <v>144</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>168</v>
       </c>
       <c r="C31" t="s">
         <v>35</v>
@@ -1761,24 +1775,21 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="4">
-        <v>45748</v>
+        <v>28</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>167</v>
       </c>
       <c r="C32" t="s">
-        <v>43</v>
-      </c>
-      <c r="D32" t="s">
-        <v>73</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>30</v>
-      </c>
-      <c r="B33" s="1" t="b">
-        <v>1</v>
+        <v>29</v>
+      </c>
+      <c r="B33" s="4">
+        <v>45748</v>
       </c>
       <c r="C33" t="s">
         <v>43</v>
@@ -1789,62 +1800,65 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>31</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
+      </c>
+      <c r="B34" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>35</v>
+        <v>43</v>
+      </c>
+      <c r="D34" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="C36" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>33</v>
-      </c>
-      <c r="B37" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C37" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>76</v>
-      </c>
-      <c r="B38" t="b">
-        <v>1</v>
+        <v>33</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="C38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B39" t="b">
         <v>1</v>
@@ -1855,7 +1869,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B40" t="b">
         <v>1</v>
@@ -1866,10 +1880,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C41" t="s">
         <v>43</v>
@@ -1877,10 +1891,10 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C42" t="s">
         <v>43</v>
@@ -1888,21 +1902,21 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>84</v>
-      </c>
-      <c r="B43" t="s">
-        <v>141</v>
+        <v>81</v>
+      </c>
+      <c r="B43" t="b">
+        <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B44" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C44" t="s">
         <v>39</v>
@@ -1910,12 +1924,23 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
+        <v>85</v>
+      </c>
+      <c r="B45" t="s">
+        <v>139</v>
+      </c>
+      <c r="C45" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
         <v>86</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>87</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1930,7 +1955,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2108,8 +2133,8 @@
       <c r="A16" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="4">
-        <v>45778</v>
+      <c r="B16" s="3" t="s">
+        <v>167</v>
       </c>
       <c r="C16" t="s">
         <v>35</v>
@@ -2308,10 +2333,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6560B172-1B59-487F-ACF4-BA38A1166E57}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2677,10 +2702,10 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B31" s="4">
-        <v>45748</v>
+        <v>144</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>168</v>
       </c>
       <c r="C31" t="s">
         <v>35</v>
@@ -2688,24 +2713,21 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>66</v>
+        <v>28</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>167</v>
       </c>
       <c r="C32" t="s">
-        <v>43</v>
-      </c>
-      <c r="D32" t="s">
-        <v>73</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>83</v>
-      </c>
-      <c r="B33" s="1" t="b">
-        <v>1</v>
+        <v>29</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="C33" t="s">
         <v>43</v>
@@ -2716,62 +2738,65 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>106</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>136</v>
+        <v>83</v>
+      </c>
+      <c r="B34" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>35</v>
+        <v>43</v>
+      </c>
+      <c r="D34" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>105</v>
-      </c>
-      <c r="B35" s="6">
-        <v>1000000</v>
+        <v>106</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="C35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>44</v>
+        <v>105</v>
+      </c>
+      <c r="B36" s="6">
+        <v>1000000</v>
       </c>
       <c r="C36" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>33</v>
-      </c>
-      <c r="B37" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C37" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>123</v>
-      </c>
-      <c r="B38" t="b">
-        <v>1</v>
+        <v>33</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="C38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B39" t="b">
         <v>1</v>
@@ -2782,7 +2807,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B40" t="b">
         <v>1</v>
@@ -2793,7 +2818,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B41" t="b">
         <v>1</v>
@@ -2804,10 +2829,10 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C42" t="s">
         <v>43</v>
@@ -2815,10 +2840,10 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
       <c r="B43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C43" t="s">
         <v>43</v>
@@ -2826,23 +2851,34 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>150</v>
-      </c>
-      <c r="B44" t="s">
-        <v>151</v>
+        <v>107</v>
+      </c>
+      <c r="B44" t="b">
+        <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B45" t="s">
         <v>151</v>
       </c>
       <c r="C45" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>153</v>
+      </c>
+      <c r="B46" t="s">
+        <v>151</v>
+      </c>
+      <c r="C46" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2853,10 +2889,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9FAF09-08A3-4B91-B541-B6D49B1C84A3}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3222,10 +3258,10 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B31" s="4">
-        <v>45748</v>
+        <v>144</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>168</v>
       </c>
       <c r="C31" t="s">
         <v>35</v>
@@ -3233,24 +3269,21 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="4">
-        <v>45748</v>
+        <v>28</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>167</v>
       </c>
       <c r="C32" t="s">
-        <v>43</v>
-      </c>
-      <c r="D32" t="s">
-        <v>73</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>30</v>
-      </c>
-      <c r="B33" s="1" t="b">
-        <v>1</v>
+        <v>29</v>
+      </c>
+      <c r="B33" s="4">
+        <v>45748</v>
       </c>
       <c r="C33" t="s">
         <v>43</v>
@@ -3261,111 +3294,125 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>31</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
+      </c>
+      <c r="B34" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>35</v>
+        <v>43</v>
+      </c>
+      <c r="D34" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="C36" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>33</v>
-      </c>
-      <c r="B37" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C37" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>83</v>
-      </c>
-      <c r="B38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C38" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>105</v>
-      </c>
-      <c r="B39">
-        <v>1000000</v>
+        <v>83</v>
+      </c>
+      <c r="B39" t="s">
+        <v>44</v>
       </c>
       <c r="C39" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>106</v>
-      </c>
-      <c r="B40" t="s">
-        <v>108</v>
+        <v>105</v>
+      </c>
+      <c r="B40">
+        <v>1000000</v>
       </c>
       <c r="C40" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>107</v>
-      </c>
-      <c r="B41" t="b">
-        <v>0</v>
+        <v>106</v>
+      </c>
+      <c r="B41" t="s">
+        <v>108</v>
       </c>
       <c r="C41" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>150</v>
-      </c>
-      <c r="B42" t="s">
-        <v>151</v>
+        <v>107</v>
+      </c>
+      <c r="B42" t="b">
+        <v>0</v>
       </c>
       <c r="C42" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
+        <v>150</v>
+      </c>
+      <c r="B43" t="s">
+        <v>151</v>
+      </c>
+      <c r="C43" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
         <v>152</v>
       </c>
-      <c r="B43" t="s">
-        <v>44</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="B44" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3378,8 +3425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F065A64-70F8-4E29-A57E-BC789E2BC90C}">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C32" sqref="A31:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3408,7 +3455,7 @@
         <v>67</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C2" t="s">
         <v>35</v>
@@ -3419,7 +3466,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C3" t="s">
         <v>35</v>
@@ -3748,7 +3795,7 @@
         <v>144</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="C31" t="s">
         <v>35</v>
@@ -3758,8 +3805,8 @@
       <c r="A32" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="4">
-        <v>45870</v>
+      <c r="B32" s="3" t="s">
+        <v>167</v>
       </c>
       <c r="C32" t="s">
         <v>35</v>
@@ -3905,7 +3952,7 @@
         <v>116</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C45" t="s">
         <v>35</v>
@@ -3941,10 +3988,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC25CABC-59C5-45BC-822F-0F71D7C65392}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:C38"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4310,10 +4357,10 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B31" s="4">
-        <v>45748</v>
+        <v>144</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>168</v>
       </c>
       <c r="C31" t="s">
         <v>35</v>
@@ -4321,81 +4368,92 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>43</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
         <v>83</v>
       </c>
-      <c r="B33" s="1" t="b">
+      <c r="B34" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C33" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
+      <c r="C34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
         <v>106</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C34" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
+      <c r="C35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
         <v>105</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B36" s="6">
         <v>1000000</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C36" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
+      <c r="B37" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C37" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
+      <c r="B38" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
         <v>150</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>151</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>